<commit_message>
Ajout 2 articles + MPD via MySqlWorkBench
</commit_message>
<xml_diff>
--- a/Livrables/MCD et MPD mediastore.xlsx
+++ b/Livrables/MCD et MPD mediastore.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="23715" windowHeight="8775" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="23715" windowHeight="8775"/>
   </bookViews>
   <sheets>
     <sheet name="MCD" sheetId="1" r:id="rId1"/>
-    <sheet name="MPD" sheetId="4" r:id="rId2"/>
+    <sheet name="MPD" sheetId="5" r:id="rId2"/>
     <sheet name="Organigramme" sheetId="2" r:id="rId3"/>
     <sheet name="Planning" sheetId="3" r:id="rId4"/>
   </sheets>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="125">
   <si>
     <t>nom</t>
   </si>
@@ -304,18 +304,12 @@
     <t>Début</t>
   </si>
   <si>
-    <t>Fin</t>
-  </si>
-  <si>
     <t>Lot 5.0 : Nouveautés (site Web marchand)</t>
   </si>
   <si>
     <t>Lot 4.0 : commande (site Web marchand)</t>
   </si>
   <si>
-    <t>nom : char</t>
-  </si>
-  <si>
     <t>Lot 10.0 : gestion des users (administration)</t>
   </si>
   <si>
@@ -350,6 +344,54 @@
   </si>
   <si>
     <t>p4</t>
+  </si>
+  <si>
+    <t>En Cours</t>
+  </si>
+  <si>
+    <t>Terminé</t>
+  </si>
+  <si>
+    <t>p0</t>
+  </si>
+  <si>
+    <t>Lot 11.0 : documentations (transverse)</t>
+  </si>
+  <si>
+    <t>Lot 0.0 : Mise en place du SGBD (transverse)</t>
+  </si>
+  <si>
+    <t>10.1 : analyse</t>
+  </si>
+  <si>
+    <t>10.2 : règles métier</t>
+  </si>
+  <si>
+    <t>10.3 : codage</t>
+  </si>
+  <si>
+    <t>10.5 : tests</t>
+  </si>
+  <si>
+    <t>10.6 : intégration au site</t>
+  </si>
+  <si>
+    <t>11.1 : analyse</t>
+  </si>
+  <si>
+    <t>11.2 : règles métier</t>
+  </si>
+  <si>
+    <t>11.3 : codage</t>
+  </si>
+  <si>
+    <t>11.5 : tests</t>
+  </si>
+  <si>
+    <t>11.6 : intégration au site</t>
+  </si>
+  <si>
+    <t>En cours</t>
   </si>
 </sst>
 </file>
@@ -379,7 +421,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -419,6 +461,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -524,7 +578,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -540,8 +594,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -550,6 +602,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -589,8 +643,14 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -800,239 +860,59 @@
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>981075</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="2" name="Connecteur droit avec flèche 1"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1381125" y="2457450"/>
-          <a:ext cx="1619250" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="arrow"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>400052</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="3" name="Connecteur droit avec flèche 2"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="4210052" y="4229100"/>
-          <a:ext cx="9523" cy="695325"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="arrow"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:colOff>272143</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>40822</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>257175</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:colOff>672193</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>164647</xdr:rowOff>
     </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="4" name="Connecteur droit avec flèche 3"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="4086225" y="5686425"/>
-          <a:ext cx="1485900" cy="1047750"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1034143" y="421822"/>
+          <a:ext cx="5734050" cy="5838825"/>
         </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
+        <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="arrow"/>
-        </a:ln>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
       </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>390525</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>390525</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>142876</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="5" name="Connecteur droit avec flèche 4"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="7248525" y="2676525"/>
-          <a:ext cx="0" cy="1085851"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="arrow"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>381002</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>390525</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="9" name="Connecteur droit avec flèche 8"/>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="4191002" y="2562225"/>
-          <a:ext cx="9523" cy="695325"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="arrow"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1327,8 +1207,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C9:K39"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1449,23 +1329,23 @@
       </c>
     </row>
     <row r="20" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="G20" s="14" t="s">
+      <c r="G20" s="12" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="21" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="G21" s="14" t="s">
+      <c r="G21" s="12" t="s">
         <v>9</v>
       </c>
       <c r="K21" s="3"/>
     </row>
     <row r="22" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="G22" s="14" t="s">
+      <c r="G22" s="12" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="23" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="G23" s="15"/>
+      <c r="G23" s="13"/>
     </row>
     <row r="25" spans="3:11" x14ac:dyDescent="0.25">
       <c r="K25" s="3" t="s">
@@ -1473,17 +1353,17 @@
       </c>
     </row>
     <row r="26" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="K26" s="14" t="s">
+      <c r="K26" s="12" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="27" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="K27" s="16" t="s">
+      <c r="K27" s="14" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="28" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="K28" s="16" t="s">
+      <c r="K28" s="14" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1491,7 +1371,7 @@
       <c r="J29" t="s">
         <v>12</v>
       </c>
-      <c r="K29" s="16" t="s">
+      <c r="K29" s="14" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1499,37 +1379,37 @@
       <c r="G30" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="K30" s="13"/>
+      <c r="K30" s="11"/>
     </row>
     <row r="31" spans="3:11" x14ac:dyDescent="0.25">
       <c r="G31" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="K31" s="13"/>
+      <c r="K31" s="11"/>
     </row>
     <row r="32" spans="3:11" x14ac:dyDescent="0.25">
       <c r="G32" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K32" s="13"/>
+      <c r="K32" s="11"/>
     </row>
     <row r="33" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G33" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="K33" s="13"/>
+      <c r="K33" s="11"/>
     </row>
     <row r="34" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G34" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K34" s="13"/>
+      <c r="K34" s="11"/>
     </row>
     <row r="35" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G35" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K35" s="13"/>
+      <c r="K35" s="11"/>
     </row>
     <row r="36" spans="7:11" x14ac:dyDescent="0.25">
       <c r="G36" s="1" t="s">
@@ -1562,203 +1442,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B5:J35"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="3.85546875" customWidth="1"/>
-    <col min="3" max="5" width="6.28515625" customWidth="1"/>
-    <col min="9" max="9" width="5.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" s="3"/>
-      <c r="F8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H8" s="3"/>
-      <c r="J8" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F9" s="1"/>
-      <c r="J9" s="1"/>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F10" s="1"/>
-      <c r="J10" s="1"/>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F11" s="1"/>
-      <c r="J11" s="1"/>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F12" s="1"/>
-      <c r="J12" s="1"/>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F13" s="2"/>
-      <c r="J13" s="2"/>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F14" s="3"/>
-      <c r="J14" s="3"/>
-    </row>
-    <row r="17" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="J17" s="3"/>
-    </row>
-    <row r="19" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F19" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F20" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F21" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J21" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F22" s="2"/>
-      <c r="J22" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="J23" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="24" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="J24" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="25" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="J25" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="26" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F26" s="3"/>
-      <c r="J26" s="1"/>
-    </row>
-    <row r="27" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F27" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J27" s="1"/>
-    </row>
-    <row r="28" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F28" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J28" s="1"/>
-    </row>
-    <row r="29" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F29" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J29" s="1"/>
-    </row>
-    <row r="30" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F30" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J30" s="2"/>
-    </row>
-    <row r="31" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F31" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="32" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F32" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="33" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F33" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="34" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F34" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="35" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F35" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -1768,8 +1459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:D60"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1934,7 +1625,7 @@
         <v>51</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
@@ -1978,61 +1669,97 @@
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B46" s="8" t="s">
+        <v>97</v>
+      </c>
       <c r="D46" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>114</v>
+      </c>
       <c r="D47" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>115</v>
+      </c>
       <c r="D48" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>116</v>
+      </c>
       <c r="D49" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>117</v>
+      </c>
       <c r="D50" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>118</v>
+      </c>
       <c r="D51" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="55" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B55" s="8" t="s">
+        <v>112</v>
+      </c>
       <c r="D55" s="6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="56" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>119</v>
+      </c>
       <c r="D56" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>120</v>
+      </c>
       <c r="D57" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="58" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>121</v>
+      </c>
       <c r="D58" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="59" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>122</v>
+      </c>
       <c r="D59" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="60" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>123</v>
+      </c>
       <c r="D60" t="s">
         <v>77</v>
       </c>
@@ -2048,24 +1775,30 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:V18"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A2:W19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" customWidth="1"/>
-    <col min="2" max="2" width="54.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="22" width="5.5703125" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="54.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="5.5703125" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="23" width="5.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C2" s="23" t="s">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="D2" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="D2" s="24"/>
       <c r="E2" s="24"/>
       <c r="F2" s="24"/>
       <c r="G2" s="24"/>
@@ -2083,53 +1816,53 @@
       <c r="S2" s="24"/>
       <c r="T2" s="24"/>
       <c r="U2" s="24"/>
-      <c r="V2" s="25"/>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C3" s="26">
+      <c r="V2" s="24"/>
+      <c r="W2" s="25"/>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="D3" s="26">
         <v>42534</v>
       </c>
-      <c r="D3" s="26"/>
       <c r="E3" s="26"/>
       <c r="F3" s="26"/>
-      <c r="G3" s="27">
+      <c r="G3" s="26"/>
+      <c r="H3" s="27">
         <v>42535</v>
       </c>
-      <c r="H3" s="28"/>
       <c r="I3" s="28"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="20">
+      <c r="J3" s="28"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="20">
         <v>42536</v>
       </c>
-      <c r="L3" s="21"/>
       <c r="M3" s="21"/>
-      <c r="N3" s="22"/>
-      <c r="O3" s="27">
+      <c r="N3" s="21"/>
+      <c r="O3" s="22"/>
+      <c r="P3" s="27">
         <v>42537</v>
       </c>
-      <c r="P3" s="28"/>
       <c r="Q3" s="28"/>
-      <c r="R3" s="29"/>
-      <c r="S3" s="20">
+      <c r="R3" s="28"/>
+      <c r="S3" s="29"/>
+      <c r="T3" s="20">
         <v>42538</v>
       </c>
-      <c r="T3" s="21"/>
       <c r="U3" s="21"/>
-      <c r="V3" s="22"/>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B4" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="C4" s="31" t="s">
+      <c r="V3" s="21"/>
+      <c r="W3" s="22"/>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="C4" s="37" t="s">
+        <v>113</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30" t="s">
-        <v>95</v>
-      </c>
-      <c r="G4" s="10"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9" t="s">
+        <v>110</v>
+      </c>
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
       <c r="J4" s="10"/>
@@ -2145,10 +1878,10 @@
       <c r="T4" s="10"/>
       <c r="U4" s="10"/>
       <c r="V4" s="10"/>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
+      <c r="W4" s="10"/>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="C5" s="34"/>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
       <c r="F5" s="10"/>
@@ -2168,12 +1901,12 @@
       <c r="T5" s="10"/>
       <c r="U5" s="10"/>
       <c r="V5" s="10"/>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B6" s="11" t="s">
+      <c r="W5" s="10"/>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="C6" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="10"/>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
       <c r="F6" s="10"/>
@@ -2193,16 +1926,17 @@
       <c r="T6" s="10"/>
       <c r="U6" s="10"/>
       <c r="V6" s="10"/>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>102</v>
-      </c>
-      <c r="B7" s="11" t="s">
+      <c r="W6" s="10"/>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="C7" s="33" t="s">
         <v>42</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>105</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
@@ -2223,21 +1957,26 @@
       <c r="T7" s="10"/>
       <c r="U7" s="10"/>
       <c r="V7" s="10"/>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>102</v>
-      </c>
-      <c r="B8" s="11" t="s">
+      <c r="W7" s="10"/>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="C8" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="C8" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
+      <c r="D8" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15" t="s">
+        <v>109</v>
+      </c>
       <c r="H8" s="10"/>
       <c r="I8" s="10"/>
       <c r="J8" s="10"/>
@@ -2253,21 +1992,26 @@
       <c r="T8" s="10"/>
       <c r="U8" s="10"/>
       <c r="V8" s="10"/>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>101</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
+      <c r="W8" s="10"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="B9" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>98</v>
+      </c>
+      <c r="D9" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30" t="s">
+        <v>109</v>
+      </c>
       <c r="H9" s="10"/>
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
@@ -2283,16 +2027,17 @@
       <c r="T9" s="10"/>
       <c r="U9" s="10"/>
       <c r="V9" s="10"/>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>101</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>108</v>
+      <c r="W9" s="10"/>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="B10" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="C10" s="33" t="s">
+        <v>96</v>
       </c>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
@@ -2313,21 +2058,26 @@
       <c r="T10" s="10"/>
       <c r="U10" s="10"/>
       <c r="V10" s="10"/>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="W10" s="10"/>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="B11" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
+      <c r="B11" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="C11" s="33" t="s">
+        <v>95</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15" t="s">
+        <v>109</v>
+      </c>
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
       <c r="J11" s="10"/>
@@ -2343,21 +2093,26 @@
       <c r="T11" s="10"/>
       <c r="U11" s="10"/>
       <c r="V11" s="10"/>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>103</v>
-      </c>
-      <c r="B12" s="11" t="s">
+      <c r="W11" s="10"/>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="B12" s="31" t="s">
+        <v>101</v>
+      </c>
+      <c r="C12" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="D12" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31" t="s">
         <v>109</v>
       </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
       <c r="H12" s="10"/>
       <c r="I12" s="10"/>
       <c r="J12" s="10"/>
@@ -2373,10 +2128,12 @@
       <c r="T12" s="10"/>
       <c r="U12" s="10"/>
       <c r="V12" s="10"/>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="W12" s="10"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A13" s="10"/>
       <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
+      <c r="C13" s="34"/>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
@@ -2396,12 +2153,14 @@
       <c r="T13" s="10"/>
       <c r="U13" s="10"/>
       <c r="V13" s="10"/>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B14" s="12" t="s">
+      <c r="W13" s="10"/>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A14" s="10"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="10"/>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
@@ -2421,16 +2180,17 @@
       <c r="T14" s="10"/>
       <c r="U14" s="10"/>
       <c r="V14" s="10"/>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>101</v>
-      </c>
-      <c r="B15" s="12" t="s">
+      <c r="W14" s="10"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="B15" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="C15" s="35" t="s">
         <v>49</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>110</v>
       </c>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
@@ -2451,16 +2211,17 @@
       <c r="T15" s="10"/>
       <c r="U15" s="10"/>
       <c r="V15" s="10"/>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>101</v>
-      </c>
-      <c r="B16" s="12" t="s">
+      <c r="W15" s="10"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="B16" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="C16" s="35" t="s">
         <v>50</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>109</v>
       </c>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
@@ -2481,16 +2242,17 @@
       <c r="T16" s="10"/>
       <c r="U16" s="10"/>
       <c r="V16" s="10"/>
-    </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>103</v>
-      </c>
-      <c r="B17" s="12" t="s">
+      <c r="W16" s="10"/>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="B17" s="31" t="s">
+        <v>101</v>
+      </c>
+      <c r="C17" s="35" t="s">
         <v>51</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>108</v>
       </c>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
@@ -2511,16 +2273,17 @@
       <c r="T17" s="10"/>
       <c r="U17" s="10"/>
       <c r="V17" s="10"/>
-    </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>103</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>107</v>
+      <c r="W17" s="10"/>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="B18" s="31" t="s">
+        <v>101</v>
+      </c>
+      <c r="C18" s="35" t="s">
+        <v>97</v>
       </c>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
@@ -2541,16 +2304,51 @@
       <c r="T18" s="10"/>
       <c r="U18" s="10"/>
       <c r="V18" s="10"/>
+      <c r="W18" s="10"/>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="B19" s="32"/>
+      <c r="C19" s="36" t="s">
+        <v>112</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="10"/>
+      <c r="N19" s="10"/>
+      <c r="O19" s="10"/>
+      <c r="P19" s="10"/>
+      <c r="Q19" s="10"/>
+      <c r="R19" s="10"/>
+      <c r="S19" s="10"/>
+      <c r="T19" s="10"/>
+      <c r="U19" s="10"/>
+      <c r="V19" s="10"/>
+      <c r="W19" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="S3:V3"/>
-    <mergeCell ref="C2:V2"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="G3:J3"/>
-    <mergeCell ref="K3:N3"/>
-    <mergeCell ref="O3:R3"/>
+    <mergeCell ref="T3:W3"/>
+    <mergeCell ref="D2:W2"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="L3:O3"/>
+    <mergeCell ref="P3:S3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="72" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ajout recherche des nouveautés
</commit_message>
<xml_diff>
--- a/Livrables/MCD et MPD mediastore.xlsx
+++ b/Livrables/MCD et MPD mediastore.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="23715" windowHeight="8775"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="23715" windowHeight="8775" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="MCD" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="124">
   <si>
     <t>nom</t>
   </si>
@@ -299,9 +299,6 @@
   </si>
   <si>
     <t>Avancement</t>
-  </si>
-  <si>
-    <t>Début</t>
   </si>
   <si>
     <t>Lot 5.0 : Nouveautés (site Web marchand)</t>
@@ -604,6 +601,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -643,14 +648,6 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1207,7 +1204,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C9:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -1470,11 +1467,11 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="19"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="27"/>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="s">
@@ -1625,7 +1622,7 @@
         <v>51</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
@@ -1670,15 +1667,15 @@
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B46" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D47" t="s">
         <v>68</v>
@@ -1686,7 +1683,7 @@
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D48" t="s">
         <v>69</v>
@@ -1694,7 +1691,7 @@
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D49" t="s">
         <v>70</v>
@@ -1702,7 +1699,7 @@
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D50" t="s">
         <v>71</v>
@@ -1710,7 +1707,7 @@
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D51" t="s">
         <v>72</v>
@@ -1718,7 +1715,7 @@
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B55" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D55" s="6" t="s">
         <v>48</v>
@@ -1726,7 +1723,7 @@
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D56" t="s">
         <v>73</v>
@@ -1734,7 +1731,7 @@
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D57" t="s">
         <v>74</v>
@@ -1742,7 +1739,7 @@
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D58" t="s">
         <v>75</v>
@@ -1750,7 +1747,7 @@
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D59" t="s">
         <v>76</v>
@@ -1758,7 +1755,7 @@
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D60" t="s">
         <v>77</v>
@@ -1780,8 +1777,8 @@
   </sheetPr>
   <dimension ref="A2:W19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P18" sqref="P18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1792,76 +1789,76 @@
     <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="5.5703125" customWidth="1"/>
     <col min="7" max="7" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="23" width="5.5703125" customWidth="1"/>
+    <col min="8" max="9" width="5.5703125" customWidth="1"/>
+    <col min="10" max="10" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="23" width="5.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="31" t="s">
         <v>93</v>
       </c>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="24"/>
-      <c r="N2" s="24"/>
-      <c r="O2" s="24"/>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="24"/>
-      <c r="R2" s="24"/>
-      <c r="S2" s="24"/>
-      <c r="T2" s="24"/>
-      <c r="U2" s="24"/>
-      <c r="V2" s="24"/>
-      <c r="W2" s="25"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="32"/>
+      <c r="S2" s="32"/>
+      <c r="T2" s="32"/>
+      <c r="U2" s="32"/>
+      <c r="V2" s="32"/>
+      <c r="W2" s="33"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="D3" s="26">
+      <c r="D3" s="34">
         <v>42534</v>
       </c>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="27">
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="35">
         <v>42535</v>
       </c>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="20">
+      <c r="I3" s="36"/>
+      <c r="J3" s="36"/>
+      <c r="K3" s="37"/>
+      <c r="L3" s="28">
         <v>42536</v>
       </c>
-      <c r="M3" s="21"/>
-      <c r="N3" s="21"/>
-      <c r="O3" s="22"/>
-      <c r="P3" s="27">
+      <c r="M3" s="29"/>
+      <c r="N3" s="29"/>
+      <c r="O3" s="30"/>
+      <c r="P3" s="35">
         <v>42537</v>
       </c>
-      <c r="Q3" s="28"/>
-      <c r="R3" s="28"/>
-      <c r="S3" s="29"/>
-      <c r="T3" s="20">
+      <c r="Q3" s="36"/>
+      <c r="R3" s="36"/>
+      <c r="S3" s="37"/>
+      <c r="T3" s="28">
         <v>42538</v>
       </c>
-      <c r="U3" s="21"/>
-      <c r="V3" s="21"/>
-      <c r="W3" s="22"/>
+      <c r="U3" s="29"/>
+      <c r="V3" s="29"/>
+      <c r="W3" s="30"/>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="C4" s="37" t="s">
-        <v>113</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>94</v>
-      </c>
+      <c r="C4" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="D4" s="9"/>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
       <c r="G4" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
@@ -1881,7 +1878,7 @@
       <c r="W4" s="10"/>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="C5" s="34"/>
+      <c r="C5" s="21"/>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
       <c r="F5" s="10"/>
@@ -1904,7 +1901,7 @@
       <c r="W5" s="10"/>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="C6" s="33" t="s">
+      <c r="C6" s="20" t="s">
         <v>45</v>
       </c>
       <c r="D6" s="10"/>
@@ -1930,21 +1927,21 @@
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="C7" s="33" t="s">
+        <v>99</v>
+      </c>
+      <c r="C7" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
       <c r="K7" s="10"/>
       <c r="L7" s="10"/>
       <c r="M7" s="10"/>
@@ -1961,25 +1958,21 @@
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="C8" s="33" t="s">
+        <v>99</v>
+      </c>
+      <c r="C8" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="16" t="s">
-        <v>94</v>
-      </c>
+      <c r="D8" s="15"/>
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
-      <c r="G8" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
       <c r="K8" s="10"/>
       <c r="L8" s="10"/>
       <c r="M8" s="10"/>
@@ -1996,21 +1989,19 @@
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="B9" s="30" t="s">
-        <v>99</v>
-      </c>
-      <c r="C9" s="33" t="s">
+        <v>104</v>
+      </c>
+      <c r="B9" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="D9" s="30" t="s">
-        <v>94</v>
-      </c>
-      <c r="E9" s="30"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="30" t="s">
-        <v>109</v>
+      <c r="C9" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17" t="s">
+        <v>108</v>
       </c>
       <c r="H9" s="10"/>
       <c r="I9" s="10"/>
@@ -2031,13 +2022,13 @@
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="B10" s="30" t="s">
-        <v>99</v>
-      </c>
-      <c r="C10" s="33" t="s">
-        <v>96</v>
+        <v>105</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>95</v>
       </c>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
@@ -2062,25 +2053,23 @@
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="C11" s="33" t="s">
-        <v>95</v>
-      </c>
-      <c r="D11" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="C11" s="20" t="s">
         <v>94</v>
       </c>
+      <c r="D11" s="16"/>
       <c r="E11" s="15"/>
       <c r="F11" s="15"/>
-      <c r="G11" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15" t="s">
+        <v>108</v>
+      </c>
       <c r="K11" s="10"/>
       <c r="L11" s="10"/>
       <c r="M11" s="10"/>
@@ -2097,21 +2086,19 @@
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="B12" s="31" t="s">
-        <v>101</v>
-      </c>
-      <c r="C12" s="33" t="s">
+        <v>106</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="C12" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="D12" s="31" t="s">
-        <v>94</v>
-      </c>
-      <c r="E12" s="31"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="31" t="s">
-        <v>109</v>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18" t="s">
+        <v>108</v>
       </c>
       <c r="H12" s="10"/>
       <c r="I12" s="10"/>
@@ -2133,7 +2120,7 @@
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
       <c r="B13" s="10"/>
-      <c r="C13" s="34"/>
+      <c r="C13" s="21"/>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
@@ -2158,7 +2145,7 @@
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
       <c r="B14" s="10"/>
-      <c r="C14" s="35" t="s">
+      <c r="C14" s="22" t="s">
         <v>44</v>
       </c>
       <c r="D14" s="10"/>
@@ -2184,12 +2171,12 @@
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="B15" s="30" t="s">
-        <v>99</v>
-      </c>
-      <c r="C15" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="C15" s="22" t="s">
         <v>49</v>
       </c>
       <c r="D15" s="10"/>
@@ -2215,12 +2202,12 @@
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="B16" s="30" t="s">
-        <v>99</v>
-      </c>
-      <c r="C16" s="35" t="s">
+        <v>106</v>
+      </c>
+      <c r="B16" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="C16" s="22" t="s">
         <v>50</v>
       </c>
       <c r="D16" s="10"/>
@@ -2246,12 +2233,12 @@
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="B17" s="31" t="s">
-        <v>101</v>
-      </c>
-      <c r="C17" s="35" t="s">
+        <v>105</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="C17" s="22" t="s">
         <v>51</v>
       </c>
       <c r="D17" s="10"/>
@@ -2277,13 +2264,13 @@
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="B18" s="31" t="s">
-        <v>101</v>
-      </c>
-      <c r="C18" s="35" t="s">
-        <v>97</v>
+        <v>104</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>96</v>
       </c>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
@@ -2308,23 +2295,21 @@
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="B19" s="19"/>
+      <c r="C19" s="23" t="s">
         <v>111</v>
       </c>
-      <c r="B19" s="32"/>
-      <c r="C19" s="36" t="s">
-        <v>112</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>94</v>
-      </c>
+      <c r="D19" s="10"/>
       <c r="E19" s="10"/>
       <c r="F19" s="10"/>
       <c r="G19" s="10"/>
-      <c r="H19" s="10" t="s">
-        <v>124</v>
-      </c>
+      <c r="H19" s="10"/>
       <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
+      <c r="J19" s="10" t="s">
+        <v>123</v>
+      </c>
       <c r="K19" s="10"/>
       <c r="L19" s="10"/>
       <c r="M19" s="10"/>

</xml_diff>

<commit_message>
Ajout rapport projet & V2 planning
</commit_message>
<xml_diff>
--- a/Livrables/MCD et MPD mediastore.xlsx
+++ b/Livrables/MCD et MPD mediastore.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="129">
   <si>
     <t>nom</t>
   </si>
@@ -401,6 +401,9 @@
   </si>
   <si>
     <t>id</t>
+  </si>
+  <si>
+    <t>TE</t>
   </si>
 </sst>
 </file>
@@ -601,7 +604,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -700,6 +703,9 @@
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -959,20 +965,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>761999</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>27214</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>13608</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>27219</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>343904</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>9145</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>223158</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>44908</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Image 2"/>
+        <xdr:cNvPr id="2" name="Image 1"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -991,8 +997,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="761999" y="408214"/>
-          <a:ext cx="7201905" cy="7030431"/>
+          <a:off x="775608" y="598719"/>
+          <a:ext cx="10877550" cy="10876189"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1293,7 +1299,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C9:K53"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="K43" sqref="K43"/>
     </sheetView>
   </sheetViews>
@@ -1576,7 +1582,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
@@ -1913,7 +1919,7 @@
   <dimension ref="A2:W19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1927,8 +1933,8 @@
     <col min="8" max="9" width="5.5703125" customWidth="1"/>
     <col min="10" max="10" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5.5703125" customWidth="1"/>
-    <col min="12" max="12" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="5.5703125" customWidth="1"/>
+    <col min="12" max="13" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.5703125" customWidth="1"/>
     <col min="15" max="15" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="16" max="23" width="5.5703125" customWidth="1"/>
   </cols>
@@ -2092,7 +2098,7 @@
       <c r="J7" s="15"/>
       <c r="K7" s="15"/>
       <c r="L7" s="15" t="s">
-        <v>108</v>
+        <v>128</v>
       </c>
       <c r="M7" s="10"/>
       <c r="N7" s="10"/>
@@ -2125,7 +2131,7 @@
       <c r="J8" s="15"/>
       <c r="K8" s="15"/>
       <c r="L8" s="15" t="s">
-        <v>108</v>
+        <v>128</v>
       </c>
       <c r="M8" s="10"/>
       <c r="N8" s="10"/>
@@ -2157,10 +2163,10 @@
       <c r="I9" s="17"/>
       <c r="J9" s="17"/>
       <c r="K9" s="17"/>
-      <c r="L9" s="17" t="s">
+      <c r="L9" s="17"/>
+      <c r="M9" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="M9" s="10"/>
       <c r="N9" s="10"/>
       <c r="O9" s="10"/>
       <c r="P9" s="10"/>
@@ -2222,7 +2228,7 @@
       <c r="J11" s="15"/>
       <c r="K11" s="15"/>
       <c r="L11" s="15" t="s">
-        <v>108</v>
+        <v>128</v>
       </c>
       <c r="M11" s="10"/>
       <c r="N11" s="10"/>
@@ -2325,10 +2331,10 @@
       <c r="A15" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="B15" s="26" t="s">
-        <v>98</v>
-      </c>
-      <c r="C15" s="17" t="s">
+      <c r="B15" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="C15" s="27" t="s">
         <v>49</v>
       </c>
       <c r="D15" s="10"/>
@@ -2339,12 +2345,12 @@
       <c r="I15" s="10"/>
       <c r="J15" s="10"/>
       <c r="K15" s="10"/>
-      <c r="L15" s="17"/>
-      <c r="M15" s="17"/>
-      <c r="N15" s="17"/>
-      <c r="O15" s="17" t="s">
+      <c r="L15" s="27"/>
+      <c r="M15" s="27" t="s">
         <v>123</v>
       </c>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
       <c r="P15" s="10"/>
       <c r="Q15" s="10"/>
       <c r="R15" s="10"/>
@@ -2368,13 +2374,11 @@
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="17"/>
-      <c r="K16" s="17"/>
-      <c r="L16" s="17" t="s">
-        <v>123</v>
-      </c>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
       <c r="M16" s="10"/>
       <c r="N16" s="10"/>
       <c r="O16" s="10"/>
@@ -2391,24 +2395,24 @@
       <c r="A17" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="B17" s="27" t="s">
-        <v>100</v>
-      </c>
-      <c r="C17" s="27" t="s">
+      <c r="B17" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="C17" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="D17" s="27"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="27"/>
-      <c r="H17" s="27"/>
-      <c r="I17" s="27"/>
-      <c r="J17" s="27"/>
-      <c r="K17" s="27"/>
-      <c r="L17" s="27" t="s">
+      <c r="D17" s="26"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="26"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="26"/>
+      <c r="M17" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="M17" s="10"/>
       <c r="N17" s="10"/>
       <c r="O17" s="10"/>
       <c r="P17" s="10"/>
@@ -2427,7 +2431,7 @@
       <c r="B18" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="C18" s="27" t="s">
+      <c r="C18" s="49" t="s">
         <v>96</v>
       </c>
       <c r="D18" s="27"/>
@@ -2438,10 +2442,10 @@
       <c r="I18" s="27"/>
       <c r="J18" s="27"/>
       <c r="K18" s="27"/>
-      <c r="L18" s="27" t="s">
+      <c r="L18" s="27"/>
+      <c r="M18" s="27" t="s">
         <v>123</v>
       </c>
-      <c r="M18" s="10"/>
       <c r="N18" s="10"/>
       <c r="O18" s="10"/>
       <c r="P18" s="10"/>
@@ -2471,10 +2475,10 @@
       <c r="I19" s="23"/>
       <c r="J19" s="23"/>
       <c r="K19" s="23"/>
-      <c r="L19" s="23" t="s">
+      <c r="L19" s="23"/>
+      <c r="M19" s="23" t="s">
         <v>123</v>
       </c>
-      <c r="M19" s="10"/>
       <c r="N19" s="10"/>
       <c r="O19" s="10"/>
       <c r="P19" s="10"/>

</xml_diff>